<commit_message>
Update the wifi calculation parameter
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91C5C97-01ED-4C55-AC56-21323EA12B42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C58A2AB-09D7-4B51-AE30-553161E1487B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="1905" windowWidth="20910" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>MAC</t>
   </si>
@@ -89,6 +89,30 @@
   </si>
   <si>
     <t>真实距离</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Sarah Office</t>
+  </si>
+  <si>
+    <t>Classroom</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Dorm</t>
+  </si>
+  <si>
+    <t>DORM</t>
   </si>
 </sst>
 </file>
@@ -633,115 +657,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0.61188057575182198</c:v>
+                  <c:v>0.24620924014946252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65062887486555709</c:v>
+                  <c:v>0.27213387683753071</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69183097091893653</c:v>
+                  <c:v>0.3007882518043099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73564225445964126</c:v>
+                  <c:v>0.33245979322709401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78222795638600262</c:v>
+                  <c:v>0.36746619407366887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83176377110267097</c:v>
+                  <c:v>0.40615859883769784</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88443651913859966</c:v>
+                  <c:v>0.44892512582186045</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.94044485172635184</c:v>
+                  <c:v>0.49619476030029025</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.54844165761210184</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.6061898993497572</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67001875035095881</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.74056846922624364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.81854673070690276</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.90473572423492965</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0633265716371612</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.130663397949639</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2022644346174129</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2783997194630237</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3593563908785258</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.4454397707459274</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5369745159352715</c:v>
+                  <c:v>1.1052951411260217</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.6343058427231376</c:v>
+                  <c:v>1.221677348996792</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.7378008287493758</c:v>
+                  <c:v>1.3503140378698733</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.8478497974222912</c:v>
+                  <c:v>1.4924955450518296</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.9648677899934677</c:v>
+                  <c:v>1.6496480740980206</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0892961308540396</c:v>
+                  <c:v>1.8233480008684413</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.221604091955812</c:v>
+                  <c:v>2.0153376859417333</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.3622906626344617</c:v>
+                  <c:v>2.227542951999558</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.5118864315095806</c:v>
+                  <c:v>2.4620924014946262</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.6709555875589852</c:v>
+                  <c:v>2.7213387683753081</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.8400980479142151</c:v>
+                  <c:v>3.0078825180431004</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.019951720402017</c:v>
+                  <c:v>3.3245979322709416</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.2111949093648224</c:v>
+                  <c:v>3.6746619407366903</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.4145488738336023</c:v>
+                  <c:v>4.0615859883769803</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.630780547701014</c:v>
+                  <c:v>4.4892512582186059</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.8607054321538139</c:v>
+                  <c:v>4.9619476030029057</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.1051906712730792</c:v>
+                  <c:v>5.4844165761210206</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.3651583224016601</c:v>
+                  <c:v>6.0618989934975751</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6415888336127793</c:v>
+                  <c:v>6.7001875035095892</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.9355247413948069</c:v>
+                  <c:v>7.4056846922624393</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.2480746024977281</c:v>
+                  <c:v>8.1854673070690307</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.5804171747699645</c:v>
+                  <c:v>9.0473572423493014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,115 +802,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0.331131121482591</c:v>
+                  <c:v>1.5016610723433851E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35210052016845189</c:v>
+                  <c:v>1.6630828608915644E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3743978389823811</c:v>
+                  <c:v>1.8418567632409181E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3981071705534972</c:v>
+                  <c:v>2.0398480533180715E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42331793280882085</c:v>
+                  <c:v>2.2591225135791232E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45012520620613355</c:v>
+                  <c:v>2.5019679887716851E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47863009232263831</c:v>
+                  <c:v>2.7709182566291082E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.50894009515180894</c:v>
+                  <c:v>3.0687794645565879E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.54116952654646366</c:v>
+                  <c:v>3.3986594081417361E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57543993733715681</c:v>
+                  <c:v>3.763999956972907E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.61188057575182198</c:v>
+                  <c:v>4.1686129660866586E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.65062887486555709</c:v>
+                  <c:v>4.616720047733755E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.69183097091893653</c:v>
+                  <c:v>5.1129966184305327E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.73564225445964126</c:v>
+                  <c:v>5.662620680869513E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.78222795638600262</c:v>
+                  <c:v>6.2713268496652694E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.83176377110267097</c:v>
+                  <c:v>6.9454661846241383E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88443651913859966</c:v>
+                  <c:v>7.6920724558204367E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.94044485172635184</c:v>
+                  <c:v>8.5189355318693288E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>9.4346826571078082E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0633265716371612</c:v>
+                  <c:v>0.10448868465705888</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.130663397949639</c:v>
+                  <c:v>0.11572074671888499</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2022644346174129</c:v>
+                  <c:v>0.12816020476406351</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2783997194630237</c:v>
+                  <c:v>0.14193684841204199</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3593563908785258</c:v>
+                  <c:v>0.15719441908064125</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4454397707459274</c:v>
+                  <c:v>0.17409210974141826</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5369745159352715</c:v>
+                  <c:v>0.19280622589196311</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6343058427231376</c:v>
+                  <c:v>0.21353202507522126</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.7378008287493758</c:v>
+                  <c:v>0.2364857541388424</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.8478497974222912</c:v>
+                  <c:v>0.26190690549071544</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.9648677899934677</c:v>
+                  <c:v>0.29006071589179028</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.0892961308540396</c:v>
+                  <c:v>0.32124093385785302</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.221604091955812</c:v>
+                  <c:v>0.35577288454450201</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3622906626344617</c:v>
+                  <c:v>0.39401686409342784</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.5118864315095806</c:v>
+                  <c:v>0.43637189885560107</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.6709555875589852</c:v>
+                  <c:v>0.48327990871398613</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.8400980479142151</c:v>
+                  <c:v>0.53523031794466081</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.019951720402017</c:v>
+                  <c:v>0.59276516172469695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,115 +947,115 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0.54116952654646366</c:v>
+                  <c:v>0.19054607179632471</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58434141337351753</c:v>
+                  <c:v>0.20892961308540398</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.22908676527677729</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25118864315095801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27542287033381663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30199517204020154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33113112148259105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.36307805477010124</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3981071705534972</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43651583224016594</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.47863009232263831</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52480746024977254</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.57543993733715693</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.63095734448019325</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.68129206905796125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.73564225445964126</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.79432823472428149</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.85769589859089412</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.92611872812879348</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="14">
+                  <c:v>0.69183097091893653</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75857757502918366</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.83176377110267097</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.91201083935590965</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0797751623277096</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.1659144011798317</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2589254117941673</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3593563908785258</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.4677992676220697</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="19">
+                  <c:v>1.0964781961431851</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2022644346174129</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3182567385564072</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4454397707459274</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>1.5848931924611136</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.7113283041617808</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.8478497974222912</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.9952623149688797</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.1544346900318838</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.3263050671536263</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.5118864315095801</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.7122725793320286</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.9286445646252366</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.1622776601683795</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.4145488738336023</c:v>
+                  <c:v>1.7378008287493756</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.6869450645195756</c:v>
+                  <c:v>1.9054607179632472</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>2.0892961308540396</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2908676527677732</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.5118864315095806</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7542287033381672</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.0199517204020165</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.3113112148259116</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.6307805477010135</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>3.9810717055349727</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.2986623470822769</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.6415888336127793</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.0118723362727238</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>5.4116952654646377</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5.8434141337351768</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.3095734448019334</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6.812920690579614</c:v>
-                </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.3564225445964153</c:v>
+                  <c:v>4.3651583224016601</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.9432823472428176</c:v>
+                  <c:v>4.7863009232263831</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.5769589859089415</c:v>
+                  <c:v>5.2480746024977263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2402,16 +2426,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2937,26 +2961,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8656B55D-6E8B-47C5-AB15-481669BCF850}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C1">
         <v>38</v>
       </c>
       <c r="D1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>3.75</v>
       </c>
@@ -2964,843 +3000,1045 @@
         <v>3.75</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-20</v>
       </c>
       <c r="B3">
-        <f>POWER(10,(ABS(A3)-28)/10/3.75)</f>
-        <v>0.61188057575182198</v>
+        <f>POWER(10,(ABS(A3)-34)/10/2.3)</f>
+        <v>0.24620924014946252</v>
       </c>
       <c r="C3">
-        <f>POWER(10,(ABS(A3)-38)/10/3.75)</f>
-        <v>0.331131121482591</v>
+        <f>POWER(10,(ABS(A3)-61.12195)/10/2.2552)</f>
+        <v>1.5016610723433851E-2</v>
       </c>
       <c r="D3">
-        <f>POWER(10,(ABS(A3)-28)/10/3)</f>
-        <v>0.54116952654646366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f>POWER(10,(ABS(A3)-38)/10/2.5)</f>
+        <v>0.19054607179632471</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>-46</v>
+      </c>
+      <c r="W3">
+        <v>-44</v>
+      </c>
+      <c r="X3">
+        <v>-43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3-1</f>
         <v>-21</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B62" si="0">POWER(10,(ABS(A4)-28)/10/3.75)</f>
-        <v>0.65062887486555709</v>
+        <f t="shared" ref="B4:B61" si="0">POWER(10,(ABS(A4)-34)/10/2.3)</f>
+        <v>0.27213387683753071</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C39" si="1">POWER(10,(ABS(A4)-38)/10/3.75)</f>
-        <v>0.35210052016845189</v>
+        <f t="shared" ref="C4:C68" si="1">POWER(10,(ABS(A4)-61.12195)/10/2.2552)</f>
+        <v>1.6630828608915644E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D39" si="2">POWER(10,(ABS(A4)-28)/10/3)</f>
-        <v>0.58434141337351753</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D4:D62" si="2">POWER(10,(ABS(A4)-38)/10/2.5)</f>
+        <v>0.20892961308540398</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>-55</v>
+      </c>
+      <c r="W4">
+        <v>-42</v>
+      </c>
+      <c r="X4">
+        <v>-44</v>
+      </c>
+      <c r="Y4">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A39" si="3">A4-1</f>
         <v>-22</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.69183097091893653</v>
+        <v>0.3007882518043099</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>0.3743978389823811</v>
+        <v>1.8418567632409181E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>0.63095734448019325</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.22908676527677729</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>-23</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.73564225445964126</v>
+        <v>0.33245979322709401</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0.3981071705534972</v>
+        <v>2.0398480533180715E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="2"/>
-        <v>0.68129206905796125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.25118864315095801</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.78222795638600262</v>
+        <v>0.36746619407366887</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0.42331793280882085</v>
+        <v>2.2591225135791232E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="2"/>
-        <v>0.73564225445964126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.27542287033381663</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>-25</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.83176377110267097</v>
+        <v>0.40615859883769784</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0.45012520620613355</v>
+        <v>2.5019679887716851E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="2"/>
-        <v>0.79432823472428149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.30199517204020154</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>-26</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.88443651913859966</v>
+        <v>0.44892512582186045</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0.47863009232263831</v>
+        <v>2.7709182566291082E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>0.85769589859089412</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.33113112148259105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>-27</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.94044485172635184</v>
+        <v>0.49619476030029025</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0.50894009515180894</v>
+        <v>3.0687794645565879E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0.92611872812879348</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.36307805477010124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>-28</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.54844165761210184</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>0.54116952654646366</v>
+        <v>3.3986594081417361E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.3981071705534972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>-29</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>1.0633265716371612</v>
+        <v>0.6061898993497572</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>0.57543993733715681</v>
+        <v>3.763999956972907E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>1.0797751623277096</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.43651583224016594</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>-30</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>1.130663397949639</v>
+        <v>0.67001875035095881</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0.61188057575182198</v>
+        <v>4.1686129660866586E-2</v>
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>1.1659144011798317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.47863009232263831</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>-31</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>1.2022644346174129</v>
+        <v>0.74056846922624364</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.65062887486555709</v>
+        <v>4.616720047733755E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>1.2589254117941673</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.52480746024977254</v>
+      </c>
+      <c r="U14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>-32</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>1.2783997194630237</v>
+        <v>0.81854673070690276</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.69183097091893653</v>
+        <v>5.1129966184305327E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="2"/>
-        <v>1.3593563908785258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.57543993733715693</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>-40</v>
+      </c>
+      <c r="W15">
+        <v>-40</v>
+      </c>
+      <c r="X15">
+        <v>-42</v>
+      </c>
+      <c r="Y15">
+        <v>-40</v>
+      </c>
+      <c r="Z15">
+        <v>-40</v>
+      </c>
+      <c r="AA15">
+        <v>-41</v>
+      </c>
+      <c r="AB15">
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>-33</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>1.3593563908785258</v>
+        <v>0.90473572423492965</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>0.73564225445964126</v>
+        <v>5.662620680869513E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="2"/>
-        <v>1.4677992676220697</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.63095734448019325</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="V16">
+        <v>-42</v>
+      </c>
+      <c r="W16">
+        <v>-40</v>
+      </c>
+      <c r="X16">
+        <v>-41</v>
+      </c>
+      <c r="Y16">
+        <v>-42</v>
+      </c>
+      <c r="Z16">
+        <v>-44</v>
+      </c>
+      <c r="AA16">
+        <v>-42</v>
+      </c>
+      <c r="AB16">
+        <v>-43</v>
+      </c>
+      <c r="AC16">
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="3"/>
         <v>-34</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>1.4454397707459274</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>0.78222795638600262</v>
+        <v>6.2713268496652694E-2</v>
       </c>
       <c r="D17">
         <f t="shared" si="2"/>
-        <v>1.5848931924611136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.69183097091893653</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
+      <c r="V17">
+        <v>-51</v>
+      </c>
+      <c r="W17">
+        <v>-53</v>
+      </c>
+      <c r="X17">
+        <v>-49</v>
+      </c>
+      <c r="Y17">
+        <v>-50</v>
+      </c>
+      <c r="Z17">
+        <v>-52</v>
+      </c>
+      <c r="AA17">
+        <v>-49</v>
+      </c>
+      <c r="AB17">
+        <v>-53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="3"/>
         <v>-35</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>1.5369745159352715</v>
+        <v>1.1052951411260217</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>0.83176377110267097</v>
+        <v>6.9454661846241383E-2</v>
       </c>
       <c r="D18">
         <f t="shared" si="2"/>
-        <v>1.7113283041617808</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.75857757502918366</v>
+      </c>
+      <c r="U18">
+        <v>4</v>
+      </c>
+      <c r="V18">
+        <v>-50</v>
+      </c>
+      <c r="W18">
+        <v>-51</v>
+      </c>
+      <c r="X18">
+        <v>-45</v>
+      </c>
+      <c r="Y18">
+        <v>-44</v>
+      </c>
+      <c r="Z18">
+        <v>-47</v>
+      </c>
+      <c r="AA18">
+        <v>-47</v>
+      </c>
+      <c r="AB18">
+        <v>-45</v>
+      </c>
+      <c r="AC18">
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="3"/>
         <v>-36</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>1.6343058427231376</v>
+        <v>1.221677348996792</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>0.88443651913859966</v>
+        <v>7.6920724558204367E-2</v>
       </c>
       <c r="D19">
         <f t="shared" si="2"/>
-        <v>1.8478497974222912</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.83176377110267097</v>
+      </c>
+      <c r="U19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="3"/>
         <v>-37</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>1.7378008287493758</v>
+        <v>1.3503140378698733</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>0.94044485172635184</v>
+        <v>8.5189355318693288E-2</v>
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>1.9952623149688797</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.91201083935590965</v>
+      </c>
+      <c r="U20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="3"/>
         <v>-38</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>1.8478497974222912</v>
+        <v>1.4924955450518296</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
+        <v>9.4346826571078082E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>2.1544346900318838</v>
-      </c>
-      <c r="F21">
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="3"/>
         <v>-39</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.9648677899934677</v>
+        <v>1.6496480740980206</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>1.0633265716371612</v>
+        <v>0.10448868465705888</v>
       </c>
       <c r="D22">
         <f t="shared" si="2"/>
-        <v>2.3263050671536263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0964781961431851</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="3"/>
         <v>-40</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>2.0892961308540396</v>
+        <v>1.8233480008684413</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>1.130663397949639</v>
+        <v>0.11572074671888499</v>
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
-        <v>2.5118864315095801</v>
-      </c>
-      <c r="F23">
-        <v>2.67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.2022644346174129</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="3"/>
         <v>-41</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>2.221604091955812</v>
+        <v>2.0153376859417333</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>1.2022644346174129</v>
+        <v>0.12816020476406351</v>
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>2.7122725793320286</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.3182567385564072</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="3"/>
         <v>-42</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>2.3622906626344617</v>
+        <v>2.227542951999558</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>1.2783997194630237</v>
+        <v>0.14193684841204199</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>2.9286445646252366</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.4454397707459274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="3"/>
         <v>-43</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>2.5118864315095806</v>
+        <v>2.4620924014946262</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>1.3593563908785258</v>
+        <v>0.15719441908064125</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>3.1622776601683795</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="H26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="3"/>
         <v>-44</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>2.6709555875589852</v>
+        <v>2.7213387683753081</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>1.4454397707459274</v>
+        <v>0.17409210974141826</v>
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>3.4145488738336023</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.7378008287493756</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="3"/>
         <v>-45</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>2.8400980479142151</v>
+        <v>3.0078825180431004</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>1.5369745159352715</v>
+        <v>0.19280622589196311</v>
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
-        <v>3.6869450645195756</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.9054607179632472</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="3"/>
         <v>-46</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>3.019951720402017</v>
+        <v>3.3245979322709416</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>1.6343058427231376</v>
+        <v>0.21353202507522126</v>
       </c>
       <c r="D29">
         <f t="shared" si="2"/>
-        <v>3.9810717055349727</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.0892961308540396</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>-47</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>3.2111949093648224</v>
+        <v>3.6746619407366903</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>1.7378008287493758</v>
+        <v>0.2364857541388424</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>4.2986623470822769</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.2908676527677732</v>
+      </c>
+      <c r="L30">
+        <v>83.673468999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>-48</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>3.4145488738336023</v>
+        <v>4.0615859883769803</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>1.8478497974222912</v>
+        <v>0.26190690549071544</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
-        <v>4.6415888336127793</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.5118864315095806</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <v>61.121951000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>-49</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3.630780547701014</v>
+        <v>4.4892512582186059</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>1.9648677899934677</v>
+        <v>0.29006071589179028</v>
       </c>
       <c r="D32">
         <f t="shared" si="2"/>
-        <v>5.0118723362727238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.7542287033381672</v>
+      </c>
+      <c r="L32">
+        <v>-82.428571000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="3"/>
         <v>-50</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>3.8607054321538139</v>
+        <v>4.9619476030029057</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>2.0892961308540396</v>
+        <v>0.32124093385785302</v>
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
-        <v>5.4116952654646377</v>
-      </c>
-      <c r="F33">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0199517204020165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="3"/>
         <v>-51</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>4.1051906712730792</v>
+        <v>5.4844165761210206</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>2.221604091955812</v>
+        <v>0.35577288454450201</v>
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
-        <v>5.8434141337351768</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.3113112148259116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="3"/>
         <v>-52</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>4.3651583224016601</v>
+        <v>6.0618989934975751</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>2.3622906626344617</v>
+        <v>0.39401686409342784</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
-        <v>6.3095734448019334</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.6307805477010135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="3"/>
         <v>-53</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>4.6415888336127793</v>
+        <v>6.7001875035095892</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>2.5118864315095806</v>
+        <v>0.43637189885560107</v>
       </c>
       <c r="D36">
         <f t="shared" si="2"/>
-        <v>6.812920690579614</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.9810717055349727</v>
+      </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="3"/>
         <v>-54</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>4.9355247413948069</v>
+        <v>7.4056846922624393</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>2.6709555875589852</v>
+        <v>0.48327990871398613</v>
       </c>
       <c r="D37">
         <f t="shared" si="2"/>
-        <v>7.3564225445964153</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.3651583224016601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>A37-1</f>
         <v>-55</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>5.2480746024977281</v>
+        <v>8.1854673070690307</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>2.8400980479142151</v>
+        <v>0.53523031794466081</v>
       </c>
       <c r="D38">
         <f t="shared" si="2"/>
-        <v>7.9432823472428176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.7863009232263831</v>
+      </c>
+      <c r="H38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>-56</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>5.5804171747699645</v>
+        <v>9.0473572423493014</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>3.019951720402017</v>
+        <v>0.59276516172469695</v>
       </c>
       <c r="D39">
         <f t="shared" si="2"/>
-        <v>8.5769589859089415</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.2480746024977263</v>
+      </c>
+      <c r="H39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" ref="A40:A54" si="4">A39-1</f>
         <v>-57</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
-        <v>5.9338058627532799</v>
+        <f>POWER(10,(ABS(A40)-34)/10/2.3)</f>
+        <v>10</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:C54" si="5">POWER(10,(ABS(A40)-38)/10/3.75)</f>
-        <v>3.2111949093648224</v>
+        <f t="shared" si="1"/>
+        <v>0.65648474156659309</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D54" si="6">POWER(10,(ABS(A40)-28)/10/3)</f>
-        <v>9.2611872812879383</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <f>POWER(10,(ABS(A40)-38)/10/2.5)</f>
+        <v>5.7543993733715713</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="4"/>
         <v>-58</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
+        <v>11.052951411260219</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0.72705388868638787</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
         <v>6.3095734448019343</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="5"/>
-        <v>3.4145488738336023</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="4"/>
         <v>-59</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>6.7091370995541135</v>
+        <v>12.216773489967926</v>
       </c>
       <c r="C42">
-        <f t="shared" si="5"/>
-        <v>3.630780547701014</v>
+        <f t="shared" si="1"/>
+        <v>0.80520890065557915</v>
       </c>
       <c r="D42">
-        <f t="shared" si="6"/>
-        <v>10.797751623277103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>6.9183097091893675</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="4"/>
         <v>-60</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>7.1340037507125631</v>
+        <v>13.50314037869874</v>
       </c>
       <c r="C43">
-        <f t="shared" si="5"/>
-        <v>3.8607054321538139</v>
+        <f t="shared" si="1"/>
+        <v>0.89176522371182143</v>
       </c>
       <c r="D43">
-        <f t="shared" si="6"/>
-        <v>11.659144011798322</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>7.585775750291841</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="4"/>
         <v>-61</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>7.5857757502918375</v>
+        <v>14.924955450518306</v>
       </c>
       <c r="C44">
-        <f t="shared" si="5"/>
-        <v>4.1051906712730792</v>
+        <f t="shared" si="1"/>
+        <v>0.9876259608833533</v>
       </c>
       <c r="D44">
-        <f t="shared" si="6"/>
-        <v>12.589254117941675</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>8.3176377110267108</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="4"/>
         <v>-62</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>8.0661569217661349</v>
+        <v>16.496480740980211</v>
       </c>
       <c r="C45">
-        <f t="shared" si="5"/>
-        <v>4.3651583224016601</v>
+        <f t="shared" si="1"/>
+        <v>1.0937912946984063</v>
       </c>
       <c r="D45">
-        <f t="shared" si="6"/>
-        <v>13.593563908785256</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>9.1201083935590983</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="4"/>
         <v>-63</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>8.5769589859089415</v>
+        <v>18.23348000868442</v>
       </c>
       <c r="C46">
-        <f t="shared" si="5"/>
-        <v>4.6415888336127793</v>
+        <f t="shared" si="1"/>
+        <v>1.2113689227933506</v>
       </c>
       <c r="D46">
-        <f t="shared" si="6"/>
-        <v>14.677992676220699</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="4"/>
         <v>-64</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>9.1201083935591036</v>
+        <v>20.153376859417335</v>
       </c>
       <c r="C47">
-        <f t="shared" si="5"/>
-        <v>4.9355247413948069</v>
+        <f t="shared" si="1"/>
+        <v>1.3415856153016255</v>
       </c>
       <c r="D47">
-        <f t="shared" si="6"/>
-        <v>15.848931924611136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10.964781961431854</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="4"/>
         <v>-65</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>9.6976535910824957</v>
+        <v>22.275429519995594</v>
       </c>
       <c r="C48">
-        <f t="shared" si="5"/>
-        <v>5.2480746024977281</v>
+        <f t="shared" si="1"/>
+        <v>1.4858000146098189</v>
       </c>
       <c r="D48">
-        <f t="shared" si="6"/>
-        <v>17.113283041617812</v>
+        <f t="shared" si="2"/>
+        <v>12.022644346174133</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,15 +4048,15 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>10.311772745930551</v>
+        <v>24.620924014946279</v>
       </c>
       <c r="C49">
-        <f t="shared" si="5"/>
-        <v>5.5804171747699645</v>
+        <f t="shared" si="1"/>
+        <v>1.6455168110297664</v>
       </c>
       <c r="D49">
-        <f t="shared" si="6"/>
-        <v>18.478497974222911</v>
+        <f t="shared" si="2"/>
+        <v>13.18256738556407</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3828,15 +4066,15 @@
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>10.964781961431854</v>
+        <v>27.21338768375308</v>
       </c>
       <c r="C50">
-        <f t="shared" si="5"/>
-        <v>5.9338058627532799</v>
+        <f t="shared" si="1"/>
+        <v>1.8224024422914273</v>
       </c>
       <c r="D50">
-        <f t="shared" si="6"/>
-        <v>19.952623149688804</v>
+        <f t="shared" si="2"/>
+        <v>14.454397707459275</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,15 +4084,15 @@
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>11.659144011798322</v>
+        <v>30.078825180431018</v>
       </c>
       <c r="C51">
-        <f t="shared" si="5"/>
-        <v>6.3095734448019343</v>
+        <f t="shared" si="1"/>
+        <v>2.0183024806603944</v>
       </c>
       <c r="D51">
-        <f t="shared" si="6"/>
-        <v>21.544346900318843</v>
+        <f t="shared" si="2"/>
+        <v>15.848931924611136</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3864,15 +4102,15 @@
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>12.397477630289442</v>
+        <v>33.245979322709424</v>
       </c>
       <c r="C52">
-        <f t="shared" si="5"/>
-        <v>6.7091370995541135</v>
+        <f t="shared" si="1"/>
+        <v>2.2352608890920735</v>
       </c>
       <c r="D52">
-        <f t="shared" si="6"/>
-        <v>23.263050671536252</v>
+        <f t="shared" si="2"/>
+        <v>17.378008287493756</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3882,15 +4120,15 @@
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>13.182567385564075</v>
+        <v>36.746619407366914</v>
       </c>
       <c r="C53">
-        <f t="shared" si="5"/>
-        <v>7.1340037507125631</v>
+        <f t="shared" si="1"/>
+        <v>2.4755413473355352</v>
       </c>
       <c r="D53">
-        <f t="shared" si="6"/>
-        <v>25.118864315095809</v>
+        <f t="shared" si="2"/>
+        <v>19.054607179632477</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3900,162 +4138,249 @@
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>14.017374183467705</v>
+        <v>40.615859883769836</v>
       </c>
       <c r="C54">
-        <f t="shared" si="5"/>
-        <v>7.5857757502918375</v>
+        <f t="shared" si="1"/>
+        <v>2.7416508704972937</v>
       </c>
       <c r="D54">
-        <f t="shared" si="6"/>
-        <v>27.122725793320289</v>
+        <f t="shared" si="2"/>
+        <v>20.892961308540393</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" ref="A55:A62" si="7">A54-1</f>
+        <f t="shared" ref="A55:A62" si="5">A54-1</f>
         <v>-72</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>14.905046433861969</v>
+        <v>44.892512582186065</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55:C62" si="8">POWER(10,(ABS(A55)-38)/10/3.75)</f>
-        <v>8.0661569217661349</v>
+        <f t="shared" si="1"/>
+        <v>3.0363659664940994</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:D62" si="9">POWER(10,(ABS(A55)-28)/10/3)</f>
-        <v>29.286445646252378</v>
+        <f t="shared" si="2"/>
+        <v>22.908676527677727</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-73</v>
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>15.848931924611136</v>
+        <v>49.619476030029077</v>
       </c>
       <c r="C56">
-        <f t="shared" si="8"/>
-        <v>8.5769589859089415</v>
+        <f t="shared" si="1"/>
+        <v>3.36276160531387</v>
       </c>
       <c r="D56">
-        <f t="shared" si="9"/>
-        <v>31.622776601683803</v>
+        <f t="shared" si="2"/>
+        <v>25.118864315095799</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-74</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>16.852590447507517</v>
+        <v>54.844165761210213</v>
       </c>
       <c r="C57">
-        <f t="shared" si="8"/>
-        <v>9.1201083935591036</v>
+        <f t="shared" si="1"/>
+        <v>3.7242433023414305</v>
       </c>
       <c r="D57">
-        <f t="shared" si="9"/>
-        <v>34.14548873833602</v>
+        <f t="shared" si="2"/>
+        <v>27.542287033381665</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-75</v>
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>17.919807223753349</v>
+        <v>60.618989934975723</v>
       </c>
       <c r="C58">
-        <f t="shared" si="8"/>
-        <v>9.6976535910824957</v>
+        <f t="shared" si="1"/>
+        <v>4.1245826504969942</v>
       </c>
       <c r="D58">
-        <f t="shared" si="9"/>
-        <v>36.869450645195769</v>
+        <f t="shared" si="2"/>
+        <v>30.199517204020164</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-76</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>19.054607179632477</v>
+        <v>67.001875035095935</v>
       </c>
       <c r="C59">
-        <f t="shared" si="8"/>
-        <v>10.311772745930551</v>
+        <f t="shared" si="1"/>
+        <v>4.5679566719191662</v>
       </c>
       <c r="D59">
-        <f t="shared" si="9"/>
-        <v>39.810717055349734</v>
+        <f t="shared" si="2"/>
+        <v>33.113112148259127</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-77</v>
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>20.26127012621145</v>
+        <v>74.056846922624445</v>
       </c>
       <c r="C60">
-        <f t="shared" si="8"/>
-        <v>10.964781961431854</v>
+        <f t="shared" si="1"/>
+        <v>5.0589913997762963</v>
       </c>
       <c r="D60">
-        <f t="shared" si="9"/>
-        <v>42.986623470822813</v>
+        <f t="shared" si="2"/>
+        <v>36.307805477010156</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-78</v>
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>21.544346900318843</v>
+        <v>81.854673070690367</v>
       </c>
       <c r="C61">
-        <f t="shared" si="8"/>
-        <v>11.659144011798322</v>
+        <f t="shared" si="1"/>
+        <v>5.6028101449258756</v>
       </c>
       <c r="D61">
-        <f t="shared" si="9"/>
-        <v>46.415888336127807</v>
+        <f t="shared" si="2"/>
+        <v>39.810717055349755</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-79</v>
       </c>
       <c r="B62">
-        <f t="shared" si="0"/>
-        <v>22.908676527677727</v>
+        <f>POWER(10,(ABS(A62)-34)/10/2.3)</f>
+        <v>90.473572423493081</v>
       </c>
       <c r="C62">
-        <f t="shared" si="8"/>
-        <v>12.397477630289442</v>
+        <f t="shared" si="1"/>
+        <v>6.2050869510219764</v>
       </c>
       <c r="D62">
-        <f t="shared" si="9"/>
-        <v>50.118723362727238</v>
+        <f t="shared" si="2"/>
+        <v>43.651583224016612</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-80</v>
+      </c>
+      <c r="B63">
+        <f>POWER(10,(ABS(A63)-34)/10/2.3)</f>
+        <v>100</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>6.8721057958055463</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>-81</v>
+      </c>
+      <c r="B64">
+        <f t="shared" ref="B64:B68" si="6">POWER(10,(ABS(A64)-34)/10/2.3)</f>
+        <v>110.52951411260221</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>7.6108261562662065</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>-82</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="6"/>
+        <v>122.16773489967929</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>8.4289556217630821</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>-83</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="6"/>
+        <v>135.03140378698743</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>9.3350303127284331</v>
+      </c>
+      <c r="F66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>-84</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="6"/>
+        <v>149.24955450518308</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>10.338503944019001</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>-82.428600000000003</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="6"/>
+        <v>127.52381727744844</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>8.8060010639107098</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="U13:Y13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add mac address for devices in excel
</commit_message>
<xml_diff>
--- a/TEST.xlsx
+++ b/TEST.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C303381-FA73-497D-9BE9-9BA676473210}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9530C-AF26-4231-AFC4-3F529886C657}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1905" windowWidth="20910" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="3510" windowWidth="20910" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>MAC</t>
   </si>
@@ -91,37 +92,31 @@
     <t>真实距离</t>
   </si>
   <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>Sarah Office</t>
-  </si>
-  <si>
-    <t>Classroom</t>
-  </si>
-  <si>
     <t>Distance</t>
-  </si>
-  <si>
-    <t>Dorm</t>
   </si>
   <si>
     <t>DORM</t>
   </si>
   <si>
-    <t>A</t>
+    <t>B0:91:22:F7:64:82</t>
   </si>
   <si>
-    <t>B</t>
+    <t>Dylan</t>
   </si>
   <si>
-    <t>(B-A)/10</t>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>B0:91:22:F7:6a:dd</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>B0:91:22:F7:6B:1D</t>
   </si>
 </sst>
 </file>
@@ -2972,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8656B55D-6E8B-47C5-AB15-481669BCF850}">
   <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,17 +2986,11 @@
       <c r="E1">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
+      <c r="F1">
+        <v>38</v>
       </c>
       <c r="U1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
@@ -3017,14 +3006,11 @@
       <c r="E2">
         <v>2.5</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
+      <c r="F2">
+        <v>2.5</v>
+      </c>
+      <c r="I2">
+        <v>78.321420000000003</v>
       </c>
       <c r="U2">
         <v>1</v>
@@ -3052,6 +3038,13 @@
       <c r="E3">
         <f>POWER(10,(ABS(A3)-76.8495)/10/1.93)</f>
         <v>1.1335222564356246E-3</v>
+      </c>
+      <c r="F3">
+        <f>POWER(10,(ABS(A3)-50.894736)/10/2.9614)</f>
+        <v>9.0521626098003405E-2</v>
+      </c>
+      <c r="I3">
+        <v>80.508769999999998</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -3080,12 +3073,16 @@
         <v>1.6630828608915644E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:E68" si="2">POWER(10,(ABS(A4)-53.8)/10/2.67)</f>
+        <f t="shared" ref="D4:D67" si="2">POWER(10,(ABS(A4)-53.8)/10/2.67)</f>
         <v>5.9092937677200488E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E67" si="3">POWER(10,(ABS(A4)-76.8495)/10/1.93)</f>
+        <f t="shared" ref="E4:F67" si="3">POWER(10,(ABS(A4)-76.8495)/10/1.93)</f>
         <v>1.2771547510823113E-3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F67" si="4">POWER(10,(ABS(A4)-50.894736)/10/2.9614)</f>
+        <v>9.7840837017245219E-2</v>
       </c>
       <c r="U4">
         <v>3</v>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A39" si="4">A4-1</f>
+        <f t="shared" ref="A5:A39" si="5">A4-1</f>
         <v>-22</v>
       </c>
       <c r="B5">
@@ -3123,6 +3120,10 @@
       <c r="E5">
         <f t="shared" si="3"/>
         <v>1.4389874119818461E-3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>0.10575184959526804</v>
       </c>
       <c r="U5">
         <v>4</v>
@@ -3130,7 +3131,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-23</v>
       </c>
       <c r="B6">
@@ -3150,10 +3151,8 @@
         <v>1.6213264446516204E-3</v>
       </c>
       <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
+        <f t="shared" si="4"/>
+        <v>0.11430251450985669</v>
       </c>
       <c r="U6">
         <v>5</v>
@@ -3161,7 +3160,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-24</v>
       </c>
       <c r="B7">
@@ -3181,10 +3180,8 @@
         <v>1.8267702818235841E-3</v>
       </c>
       <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
+        <f t="shared" si="4"/>
+        <v>0.12354455145019613</v>
       </c>
       <c r="U7">
         <v>6</v>
@@ -3192,7 +3189,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-25</v>
       </c>
       <c r="B8">
@@ -3211,8 +3208,9 @@
         <f t="shared" si="3"/>
         <v>2.0582466125573296E-3</v>
       </c>
-      <c r="G8" t="s">
-        <v>31</v>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>0.13353386194941452</v>
       </c>
       <c r="U8">
         <v>7</v>
@@ -3220,7 +3218,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-26</v>
       </c>
       <c r="B9">
@@ -3238,11 +3236,15 @@
       <c r="E9">
         <f t="shared" si="3"/>
         <v>2.3190541034391735E-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>0.14433086751149476</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-27</v>
       </c>
       <c r="B10">
@@ -3260,11 +3262,15 @@
       <c r="E10">
         <f t="shared" si="3"/>
         <v>2.6129094064175351E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0.15600087507775393</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-28</v>
       </c>
       <c r="B11">
@@ -3282,11 +3288,15 @@
       <c r="E11">
         <f t="shared" si="3"/>
         <v>2.9440001231624143E-3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>0.168614472043458</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-29</v>
       </c>
       <c r="B12">
@@ -3304,11 +3314,15 @@
       <c r="E12">
         <f t="shared" si="3"/>
         <v>3.3170444807206359E-3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>0.18224795321387521</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-30</v>
       </c>
       <c r="B13">
@@ -3327,8 +3341,12 @@
         <f t="shared" si="3"/>
         <v>3.7373585688780975E-3</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>0.19698378228226068</v>
+      </c>
       <c r="U13" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
@@ -3337,7 +3355,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-31</v>
       </c>
       <c r="B14">
@@ -3356,13 +3374,17 @@
         <f t="shared" si="3"/>
         <v>4.2109320973989488E-3</v>
       </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>0.2129110906210763</v>
+      </c>
       <c r="U14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-32</v>
       </c>
       <c r="B15">
@@ -3380,6 +3402,10 @@
       <c r="E15">
         <f t="shared" si="3"/>
         <v>4.7445137527244519E-3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>0.23012621640344275</v>
       </c>
       <c r="U15">
         <v>1</v>
@@ -3408,7 +3434,7 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-33</v>
       </c>
       <c r="B16">
@@ -3426,6 +3452,10 @@
       <c r="E16">
         <f t="shared" si="3"/>
         <v>5.3457073705120775E-3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>0.24873328731576078</v>
       </c>
       <c r="U16">
         <v>2</v>
@@ -3457,7 +3487,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-34</v>
       </c>
       <c r="B17">
@@ -3475,6 +3505,10 @@
       <c r="E17">
         <f t="shared" si="3"/>
         <v>6.0230802945270383E-3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>0.26884485038610861</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -3506,7 +3540,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-35</v>
       </c>
       <c r="B18">
@@ -3524,6 +3558,10 @@
       <c r="E18">
         <f t="shared" si="3"/>
         <v>6.786285466060739E-3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="4"/>
+        <v>0.29058255273800376</v>
       </c>
       <c r="U18">
         <v>4</v>
@@ -3555,7 +3593,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-36</v>
       </c>
       <c r="B19">
@@ -3573,6 +3611,10 @@
       <c r="E19">
         <f t="shared" si="3"/>
         <v>7.6461989837184495E-3</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>0.31407787738714943</v>
       </c>
       <c r="U19">
         <v>5</v>
@@ -3580,7 +3622,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-37</v>
       </c>
       <c r="B20">
@@ -3598,6 +3640,10 @@
       <c r="E20">
         <f t="shared" si="3"/>
         <v>8.6150750938796105E-3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>0.33947293853171534</v>
       </c>
       <c r="U20">
         <v>6</v>
@@ -3605,7 +3651,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-38</v>
       </c>
       <c r="B21">
@@ -3623,6 +3669,10 @@
       <c r="E21">
         <f t="shared" si="3"/>
         <v>9.7067208205312439E-3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="4"/>
+        <v>0.36692134114656022</v>
       </c>
       <c r="U21">
         <v>7</v>
@@ -3630,7 +3680,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-39</v>
       </c>
       <c r="B22">
@@ -3648,11 +3698,15 @@
       <c r="E22">
         <f t="shared" si="3"/>
         <v>1.0936692723046785E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="4"/>
+        <v>0.39658911008075082</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-40</v>
       </c>
       <c r="B23">
@@ -3670,6 +3724,10 @@
       <c r="E23">
         <f t="shared" si="3"/>
         <v>1.2322518585818199E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="4"/>
+        <v>0.42865569427813144</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -3677,7 +3735,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-41</v>
       </c>
       <c r="B24">
@@ -3695,11 +3753,15 @@
       <c r="E24">
         <f t="shared" si="3"/>
         <v>1.388394719894199E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="4"/>
+        <v>0.46331505219508895</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-42</v>
       </c>
       <c r="B25">
@@ -3717,11 +3779,15 @@
       <c r="E25">
         <f t="shared" si="3"/>
         <v>1.5643229789473273E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="4"/>
+        <v>0.5007768249807879</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-43</v>
       </c>
       <c r="B26">
@@ -3739,6 +3805,10 @@
       <c r="E26">
         <f t="shared" si="3"/>
         <v>1.7625437113799432E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>0.54126760451599432</v>
       </c>
       <c r="H26">
         <v>3</v>
@@ -3746,7 +3816,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-44</v>
       </c>
       <c r="B27">
@@ -3764,11 +3834,15 @@
       <c r="E27">
         <f t="shared" si="3"/>
         <v>1.9858816729876775E-2</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="4"/>
+        <v>0.58503230398036599</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-45</v>
       </c>
       <c r="B28">
@@ -3786,11 +3860,15 @@
       <c r="E28">
         <f t="shared" si="3"/>
         <v>2.2375195540658043E-2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>0.63233563923824598</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-46</v>
       </c>
       <c r="B29">
@@ -3808,6 +3886,10 @@
       <c r="E29">
         <f t="shared" si="3"/>
         <v>2.5210433345178966E-2</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="4"/>
+        <v>0.68346373000329275</v>
       </c>
       <c r="H29">
         <v>4</v>
@@ -3815,7 +3897,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-47</v>
       </c>
       <c r="B30">
@@ -3833,6 +3915,10 @@
       <c r="E30">
         <f t="shared" si="3"/>
         <v>2.8404933860659343E-2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="4"/>
+        <v>0.73872583046677742</v>
       </c>
       <c r="L30">
         <v>83.673468999999997</v>
@@ -3840,7 +3926,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-48</v>
       </c>
       <c r="B31">
@@ -3858,6 +3944,10 @@
       <c r="E31">
         <f t="shared" si="3"/>
         <v>3.2004220497967958E-2</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="4"/>
+        <v>0.79845619985745386</v>
       </c>
       <c r="H31">
         <v>5</v>
@@ -3868,7 +3958,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-49</v>
       </c>
       <c r="B32">
@@ -3886,6 +3976,10 @@
       <c r="E32">
         <f t="shared" si="3"/>
         <v>3.6059585095572437E-2</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>0.8630161242472999</v>
       </c>
       <c r="L32">
         <v>-82.428571000000005</v>
@@ -3893,7 +3987,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-50</v>
       </c>
       <c r="B33">
@@ -3911,11 +4005,15 @@
       <c r="E33">
         <f t="shared" si="3"/>
         <v>4.0628818856793904E-2</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>0.93279610183225792</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-51</v>
       </c>
       <c r="B34">
@@ -3933,11 +4031,15 @@
       <c r="E34">
         <f t="shared" si="3"/>
         <v>4.5777035906629217E-2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>1.0082182049058954</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-52</v>
       </c>
       <c r="B35">
@@ -3955,11 +4057,15 @@
       <c r="E35">
         <f t="shared" si="3"/>
         <v>5.1577601204284257E-2</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>1.0897386328126628</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-53</v>
       </c>
       <c r="B36">
@@ -3977,6 +4083,10 @@
       <c r="E36">
         <f t="shared" si="3"/>
         <v>5.8113176034688185E-2</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>1.1778504713225773</v>
       </c>
       <c r="H36">
         <v>7</v>
@@ -3984,7 +4094,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-54</v>
       </c>
       <c r="B37">
@@ -4002,6 +4112,10 @@
       <c r="E37">
         <f t="shared" si="3"/>
         <v>6.5476895977824898E-2</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>1.2730866751177332</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4025,13 +4139,17 @@
         <f t="shared" si="3"/>
         <v>7.377369814260068E-2</v>
       </c>
+      <c r="F38">
+        <f t="shared" si="4"/>
+        <v>1.3760232914305564</v>
+      </c>
       <c r="H38">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-56</v>
       </c>
       <c r="B39">
@@ -4049,6 +4167,10 @@
       <c r="E39">
         <f t="shared" si="3"/>
         <v>8.3121816579069405E-2</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>1.4872829443323479</v>
       </c>
       <c r="H39">
         <v>9</v>
@@ -4056,7 +4178,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" ref="A40:A54" si="5">A39-1</f>
+        <f t="shared" ref="A40:A54" si="6">A39-1</f>
         <v>-57</v>
       </c>
       <c r="B40">
@@ -4075,10 +4197,14 @@
         <f t="shared" si="3"/>
         <v>9.3654467179471748E-2</v>
       </c>
+      <c r="F40">
+        <f t="shared" si="4"/>
+        <v>1.6075386007472474</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-58</v>
       </c>
       <c r="B41">
@@ -4096,11 +4222,15 @@
       <c r="E41">
         <f t="shared" si="3"/>
         <v>0.10552174607886738</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>1.7375176409707804</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-59</v>
       </c>
       <c r="B42">
@@ -4118,11 +4248,15 @@
       <c r="E42">
         <f t="shared" si="3"/>
         <v>0.11889276860862463</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>1.8780062583140034</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-60</v>
       </c>
       <c r="B43">
@@ -4140,11 +4274,15 @@
       <c r="E43">
         <f t="shared" si="3"/>
         <v>0.13395807928404665</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>2.0298542144849931</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-61</v>
       </c>
       <c r="B44">
@@ -4164,12 +4302,13 @@
         <v>0.15093236716979941</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2.1939799794711718</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-62</v>
       </c>
       <c r="B45">
@@ -4187,11 +4326,15 @@
       <c r="E45">
         <f t="shared" si="3"/>
         <v>0.17005752531861004</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>2.3713762870116262</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-63</v>
       </c>
       <c r="B46">
@@ -4209,11 +4352,15 @@
       <c r="E46">
         <f t="shared" si="3"/>
         <v>0.19160609788194147</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="4"/>
+        <v>2.5631161392623523</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-64</v>
       </c>
       <c r="B47">
@@ -4231,11 +4378,15 @@
       <c r="E47">
         <f t="shared" si="3"/>
         <v>0.21588516401588775</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="4"/>
+        <v>2.7703592969743389</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-65</v>
       </c>
       <c r="B48">
@@ -4254,10 +4405,14 @@
         <f t="shared" si="3"/>
         <v>0.24324071393011412</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="4"/>
+        <v>2.9943592944410762</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-66</v>
       </c>
       <c r="B49">
@@ -4276,10 +4431,14 @@
         <f t="shared" si="3"/>
         <v>0.27406257944097251</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>3.2364710216462274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-67</v>
       </c>
       <c r="B50">
@@ -4298,10 +4457,14 @@
         <f t="shared" si="3"/>
         <v>0.30878998929192175</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="4"/>
+        <v>3.4981589194729477</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-68</v>
       </c>
       <c r="B51">
@@ -4320,10 +4483,14 @@
         <f t="shared" si="3"/>
         <v>0.34791782840766072</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>3.7810058375445439</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-69</v>
       </c>
       <c r="B52">
@@ -4342,10 +4509,14 @@
         <f t="shared" si="3"/>
         <v>0.3920036902798299</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="4"/>
+        <v>4.0867226082741368</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-70</v>
       </c>
       <c r="B53">
@@ -4364,10 +4535,14 @@
         <f t="shared" si="3"/>
         <v>0.44167582298470448</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>4.4171583950330788</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-71</v>
       </c>
       <c r="B54">
@@ -4386,10 +4561,14 @@
         <f t="shared" si="3"/>
         <v>0.49764208206805643</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>4.7743118770302404</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" ref="A55:A99" si="6">A54-1</f>
+        <f t="shared" ref="A55:A82" si="7">A54-1</f>
         <v>-72</v>
       </c>
       <c r="B55">
@@ -4408,10 +4587,14 @@
         <f t="shared" si="3"/>
         <v>0.56070001788077573</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="4"/>
+        <v>5.1603433385551725</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-73</v>
       </c>
       <c r="B56">
@@ -4430,10 +4613,14 @@
         <f t="shared" si="3"/>
         <v>0.63174824111540417</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="4"/>
+        <v>5.5775877357083852</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-74</v>
       </c>
       <c r="B57">
@@ -4452,10 +4639,14 @@
         <f t="shared" si="3"/>
         <v>0.71179922850880062</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>6.0285688196543186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-75</v>
       </c>
       <c r="B58">
@@ -4474,10 +4665,14 @@
         <f t="shared" si="3"/>
         <v>0.80199375119933303</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="4"/>
+        <v>6.516014401823198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-76</v>
       </c>
       <c r="B59">
@@ -4496,10 +4691,14 @@
         <f t="shared" si="3"/>
         <v>0.90361713135071942</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="4"/>
+        <v>7.042872853395064</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-77</v>
       </c>
       <c r="B60">
@@ -4518,10 +4717,14 @@
         <f t="shared" si="3"/>
         <v>1.0181175587084581</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="4"/>
+        <v>7.6123309388650755</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-78</v>
       </c>
       <c r="B61">
@@ -4540,10 +4743,14 @@
         <f t="shared" si="3"/>
         <v>1.1471267281099728</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="4"/>
+        <v>8.227833091558427</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-79</v>
       </c>
       <c r="B62">
@@ -4562,10 +4769,14 @@
         <f t="shared" si="3"/>
         <v>1.2924830920444865</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="4"/>
+        <v>8.8931022476851069</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-80</v>
       </c>
       <c r="B63">
@@ -4584,14 +4795,18 @@
         <f t="shared" si="3"/>
         <v>1.45625805962454</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="4"/>
+        <v>9.6121623649516792</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-81</v>
       </c>
       <c r="B64">
-        <f t="shared" ref="B64:B68" si="7">POWER(10,(ABS(A64)-34)/10/2.3)</f>
+        <f t="shared" ref="B64:B68" si="8">POWER(10,(ABS(A64)-34)/10/2.3)</f>
         <v>110.52951411260221</v>
       </c>
       <c r="C64">
@@ -4605,15 +4820,19 @@
       <c r="E64">
         <f t="shared" si="3"/>
         <v>1.6407855153190951</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="4"/>
+        <v>10.389362761936503</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-82</v>
       </c>
       <c r="B65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>122.16773489967929</v>
       </c>
       <c r="C65">
@@ -4627,15 +4846,19 @@
       <c r="E65">
         <f t="shared" si="3"/>
         <v>1.8486950781065961</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="4"/>
+        <v>11.229404425447976</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-83</v>
       </c>
       <c r="B66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>135.03140378698743</v>
       </c>
       <c r="C66">
@@ -4651,16 +4874,17 @@
         <v>2.0829495750094393</v>
       </c>
       <c r="F66">
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>12.137368444988876</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-84</v>
       </c>
       <c r="B67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>149.24955450518308</v>
       </c>
       <c r="C67">
@@ -4676,16 +4900,17 @@
         <v>2.346887263028584</v>
       </c>
       <c r="F67">
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>13.118746746315956</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-85</v>
       </c>
       <c r="B68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>164.96480740980221</v>
       </c>
       <c r="C68">
@@ -4693,160 +4918,220 @@
         <v>11.449846462175675</v>
       </c>
       <c r="D68">
-        <f t="shared" ref="D68:E72" si="8">POWER(10,(ABS(A68)-53.8)/10/2.67)</f>
+        <f t="shared" ref="D68" si="9">POWER(10,(ABS(A68)-53.8)/10/2.67)</f>
         <v>14.741420201106219</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E83" si="9">POWER(10,(ABS(A68)-76.8495)/10/1.93)</f>
+        <f t="shared" ref="E68:F83" si="10">POWER(10,(ABS(A68)-76.8495)/10/1.93)</f>
         <v>2.6442694011643741</v>
+      </c>
+      <c r="F68">
+        <f t="shared" ref="F68:F82" si="11">POWER(10,(ABS(A68)-50.894736)/10/2.9614)</f>
+        <v>14.179475309990336</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-86</v>
       </c>
       <c r="E69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.9793338504513569</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="11"/>
+        <v>15.325970075844864</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-87</v>
       </c>
       <c r="E70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.3568554658374343</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="11"/>
+        <v>16.565165750540899</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-88</v>
       </c>
       <c r="E71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.7822141405252494</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="11"/>
+        <v>17.904557752946431</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-89</v>
       </c>
       <c r="E72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.2614714724455514</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="11"/>
+        <v>19.352247551047089</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-90</v>
       </c>
       <c r="E73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.8014571454024786</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="11"/>
+        <v>20.916991664615544</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-91</v>
       </c>
       <c r="E74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4098662558701625</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="11"/>
+        <v>22.608254630037692</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-92</v>
       </c>
       <c r="E75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.0953689724016877</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="11"/>
+        <v>24.436266247659546</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-93</v>
       </c>
       <c r="E76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.8677340903580575</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="11"/>
+        <v>26.412083457921923</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-94</v>
       </c>
       <c r="E77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.7379682426808047</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="11"/>
+        <v>28.547657220548047</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-95</v>
       </c>
       <c r="E78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.7184727505393198</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="11"/>
+        <v>30.855904801310615</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-96</v>
       </c>
       <c r="E79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.8232203490618808</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="11"/>
+        <v>33.350787903612947</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-97</v>
       </c>
       <c r="E80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.067954306590478</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="11"/>
+        <v>36.047397117472684</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-98</v>
       </c>
       <c r="E81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.470412775019694</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f t="shared" si="11"/>
+        <v>38.962043196706958</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-99</v>
       </c>
       <c r="E82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.050581568336828</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f t="shared" si="11"/>
+        <v>42.112355716419842</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>-83.034999999999997</v>
       </c>
       <c r="E83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0916654748683627</v>
       </c>
     </row>
@@ -4857,4 +5142,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704F796D-A82B-4DCB-BC76-574CF9E43865}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>